<commit_message>
2.7 Hind and Syria updates
Added range on Cyprus
Added Hinds to FARPs and Range
Carrier spawns are back to group per aircraft
... more
</commit_message>
<xml_diff>
--- a/Blackpool To-Do List.xlsx
+++ b/Blackpool To-Do List.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
   <si>
     <t>Task</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>What is this???</t>
+  </si>
+  <si>
+    <t>Add "Admin" Menu to Blackpool with BASECAP options, AIRBOSS start/stop, more?</t>
   </si>
 </sst>
 </file>
@@ -1103,7 +1106,7 @@
   <dimension ref="B1:F44"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1225,11 +1228,19 @@
       </c>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="4"/>
+    <row r="9" spans="2:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="4">
+        <v>1</v>
+      </c>
       <c r="F9" s="3"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.3">

</xml_diff>